<commit_message>
Made changes to the higestcand method.Add support for reading application .csv form MVC
</commit_message>
<xml_diff>
--- a/election/Meath_2002_General_format.csv.xlsx
+++ b/election/Meath_2002_General_format.csv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\philo\stvElection\election\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A1177A66-4834-42B5-AD6E-538974C292D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3D78C1-398D-4D92-9158-B271F69E7B40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meath_2002_General" sheetId="1" r:id="rId1"/>
@@ -184,7 +184,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1087,16 +1087,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J44" sqref="A7:J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="10" width="6.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>